<commit_message>
tons of new research and supplemental derivations and revised theories and equations where necessary still needs a bit of organization love but pretty robust
</commit_message>
<xml_diff>
--- a/public/spreadsheets/figure_3b_tension_detailed_complete_data.xlsx
+++ b/public/spreadsheets/figure_3b_tension_detailed_complete_data.xlsx
@@ -7,10 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Panel_A_All_H0_Measurements" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Panel_B_All_Sigma8_Measurements" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Panel_C_Expansion_History" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Panel_D_Growth_Rate_Data" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Expansion_History" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Growth_Rate_Data" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,524 +426,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Survey</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>H0_Value</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>H0_Error_Lower</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>H0_Error_Upper</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Method</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Color</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Planck CMB</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>67.36</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>CMB</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>2020</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>red</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>SH0ES</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>73.04000000000001</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1.04</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.04</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Cepheids</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>2022</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>blue</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>TRGB</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>69.8</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>TRGB</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>2021</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>cyan</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>JWST</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>68.5</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>JWST Cal</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>2023</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>lightblue</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>SPT</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>67.90000000000001</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>CMB</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>2021</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>yellow</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>ACT</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>67.2</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>CMB</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>2020</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>yellow</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>WMAP</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>68</v>
-      </c>
-      <c r="C8" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>CMB</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>2013</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>orange</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Spin-Torsion</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>68.09999999999999</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Theory</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>2025</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>green</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Survey</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Sigma8_Value</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Sigma8_Error_Lower</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Sigma8_Error_Upper</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Method</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Color</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Planck CMB</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.8111</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.0056</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.0056</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>CMB</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>2020</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>red</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>KiDS</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0.766</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Weak Lensing</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>2021</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>blue</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>DES Y3</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.773</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.016</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.016</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Weak Lensing</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>2022</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>cyan</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>HSC</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.018</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.018</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Weak Lensing</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>2019</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>lightblue</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>CFHTLenS</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.756</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Weak Lensing</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>2013</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>purple</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Spin-Torsion</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.823</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Theory</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>2025</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>green</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -962,17 +442,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>H_LCDM</t>
+          <t>H_LCDM_km_s_Mpc</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>H_Spin_Torsion</t>
+          <t>H_SpinTorsion_km_s_Mpc</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>H_Difference</t>
+          <t>Relative_Difference_Percent</t>
         </is>
       </c>
     </row>
@@ -981,13 +461,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>67.36</v>
+        <v>67.40000000000001</v>
       </c>
       <c r="C2" t="n">
-        <v>70.39379436427618</v>
+        <v>69.89200000000001</v>
       </c>
       <c r="D2" t="n">
-        <v>3.033794364276176</v>
+        <v>3.697329376854606</v>
       </c>
     </row>
     <row r="3">
@@ -995,13 +475,13 @@
         <v>0.06122448979591837</v>
       </c>
       <c r="B3" t="n">
-        <v>69.39949178576919</v>
+        <v>69.44070288540443</v>
       </c>
       <c r="C3" t="n">
-        <v>72.30257789948251</v>
+        <v>71.96581363943724</v>
       </c>
       <c r="D3" t="n">
-        <v>2.903086113713329</v>
+        <v>3.636355407000864</v>
       </c>
     </row>
     <row r="4">
@@ -1009,13 +489,13 @@
         <v>0.1224489795918367</v>
       </c>
       <c r="B4" t="n">
-        <v>71.61928935506744</v>
+        <v>71.66181862428067</v>
       </c>
       <c r="C4" t="n">
-        <v>74.40036508696336</v>
+        <v>74.2265969443164</v>
       </c>
       <c r="D4" t="n">
-        <v>2.781075731895925</v>
+        <v>3.579002555716221</v>
       </c>
     </row>
     <row r="5">
@@ -1023,13 +503,13 @@
         <v>0.1836734693877551</v>
       </c>
       <c r="B5" t="n">
-        <v>74.01646517554806</v>
+        <v>74.06041794584235</v>
       </c>
       <c r="C5" t="n">
-        <v>76.68462804132766</v>
+        <v>76.67108898357407</v>
       </c>
       <c r="D5" t="n">
-        <v>2.668162865779593</v>
+        <v>3.525055772222089</v>
       </c>
     </row>
     <row r="6">
@@ -1037,13 +517,13 @@
         <v>0.2448979591836735</v>
       </c>
       <c r="B6" t="n">
-        <v>76.58721213411151</v>
+        <v>76.63269147623392</v>
       </c>
       <c r="C6" t="n">
-        <v>79.1518058692175</v>
+        <v>79.29515086767657</v>
       </c>
       <c r="D6" t="n">
-        <v>2.564593735105987</v>
+        <v>3.474312777162943</v>
       </c>
     </row>
     <row r="7">
@@ -1051,13 +531,13 @@
         <v>0.3061224489795918</v>
       </c>
       <c r="B7" t="n">
-        <v>79.32706044080628</v>
+        <v>79.37416677123431</v>
       </c>
       <c r="C7" t="n">
-        <v>81.79752888746985</v>
+        <v>82.09398871761599</v>
       </c>
       <c r="D7" t="n">
-        <v>2.470468446663574</v>
+        <v>3.426583304137879</v>
       </c>
     </row>
     <row r="8">
@@ -1065,13 +545,13 @@
         <v>0.3673469387755102</v>
       </c>
       <c r="B8" t="n">
-        <v>82.23107416586835</v>
+        <v>82.27990497000486</v>
       </c>
       <c r="C8" t="n">
-        <v>84.61682947028277</v>
+        <v>85.06235496061441</v>
       </c>
       <c r="D8" t="n">
-        <v>2.385755304414417</v>
+        <v>3.381688386275958</v>
       </c>
     </row>
     <row r="9">
@@ -1079,13 +559,13 @@
         <v>0.4285714285714285</v>
       </c>
       <c r="B9" t="n">
-        <v>85.29402240270214</v>
+        <v>85.34467205971087</v>
       </c>
       <c r="C9" t="n">
-        <v>87.60433183674623</v>
+        <v>88.19472297659421</v>
       </c>
       <c r="D9" t="n">
-        <v>2.310309434044086</v>
+        <v>3.339459685180245</v>
       </c>
     </row>
     <row r="10">
@@ -1093,13 +573,13 @@
         <v>0.4897959183673469</v>
       </c>
       <c r="B10" t="n">
-        <v>88.51052304634342</v>
+        <v>88.56308273936382</v>
       </c>
       <c r="C10" t="n">
-        <v>90.75441639409703</v>
+        <v>91.48543319588485</v>
       </c>
       <c r="D10" t="n">
-        <v>2.243893347753612</v>
+        <v>3.299738859724818</v>
       </c>
     </row>
     <row r="11">
@@ -1107,13 +587,13 @@
         <v>0.5510204081632653</v>
       </c>
       <c r="B11" t="n">
-        <v>91.87515948102659</v>
+        <v>91.92971717668041</v>
       </c>
       <c r="C11" t="n">
-        <v>94.06135704864263</v>
+        <v>94.92881110058715</v>
       </c>
       <c r="D11" t="n">
-        <v>2.186197567616048</v>
+        <v>3.262376972337205</v>
       </c>
     </row>
     <row r="12">
@@ -1121,13 +601,13 @@
         <v>0.6122448979591837</v>
       </c>
       <c r="B12" t="n">
-        <v>95.38257205113845</v>
+        <v>95.43921253335409</v>
       </c>
       <c r="C12" t="n">
-        <v>97.51943202271144</v>
+        <v>98.51925918327161</v>
       </c>
       <c r="D12" t="n">
-        <v>2.136859971572989</v>
+        <v>3.227233930540977</v>
       </c>
     </row>
     <row r="13">
@@ -1135,13 +615,13 @@
         <v>0.673469387755102</v>
       </c>
       <c r="B13" t="n">
-        <v>99.02752712500983</v>
+        <v>99.08633206985841</v>
       </c>
       <c r="C13" t="n">
-        <v>101.1230101584837</v>
+        <v>102.2513258518544</v>
       </c>
       <c r="D13" t="n">
-        <v>2.09548303347384</v>
+        <v>3.194177961663328</v>
       </c>
     </row>
     <row r="14">
@@ -1149,13 +629,13 @@
         <v>0.7346938775510203</v>
       </c>
       <c r="B14" t="n">
-        <v>102.8049669819193</v>
+        <v>102.8660150620748</v>
       </c>
       <c r="C14" t="n">
-        <v>104.8666155291185</v>
+        <v>106.1197546767436</v>
       </c>
       <c r="D14" t="n">
-        <v>2.061648547199297</v>
+        <v>3.163085118739441</v>
       </c>
     </row>
     <row r="15">
@@ -1163,13 +643,13 @@
         <v>0.7959183673469388</v>
       </c>
       <c r="B15" t="n">
-        <v>106.7100438025638</v>
+        <v>106.7734108119478</v>
       </c>
       <c r="C15" t="n">
-        <v>108.7449735402714</v>
+        <v>110.119517404883</v>
       </c>
       <c r="D15" t="n">
-        <v>2.034929737707529</v>
+        <v>3.133838815759541</v>
       </c>
     </row>
     <row r="16">
@@ -1177,13 +657,13 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="B16" t="n">
-        <v>110.7381408519528</v>
+        <v>110.8038998429575</v>
       </c>
       <c r="C16" t="n">
-        <v>112.7530417254315</v>
+        <v>114.2458339496183</v>
       </c>
       <c r="D16" t="n">
-        <v>2.014900873478723</v>
+        <v>3.106329390516987</v>
       </c>
     </row>
     <row r="17">
@@ -1191,13 +671,13 @@
         <v>0.9183673469387755</v>
       </c>
       <c r="B17" t="n">
-        <v>114.8848836158903</v>
+        <v>114.9531050432157</v>
       </c>
       <c r="C17" t="n">
-        <v>116.8860282374061</v>
+        <v>118.494182213218</v>
       </c>
       <c r="D17" t="n">
-        <v>2.001144621515778</v>
+        <v>3.080453693417938</v>
       </c>
     </row>
     <row r="18">
@@ -1205,13 +685,13 @@
         <v>0.9795918367346939</v>
       </c>
       <c r="B18" t="n">
-        <v>119.1461432648656</v>
+        <v>119.2168951314125</v>
       </c>
       <c r="C18" t="n">
-        <v>121.1394007128006</v>
+        <v>122.8603001892543</v>
       </c>
       <c r="D18" t="n">
-        <v>1.993257447934965</v>
+        <v>3.056114700710585</v>
       </c>
     </row>
     <row r="19">
@@ -1219,13 +699,13 @@
         <v>1.040816326530612</v>
       </c>
       <c r="B19" t="n">
-        <v>123.5180344240882</v>
+        <v>123.5913824255277</v>
       </c>
       <c r="C19" t="n">
-        <v>125.5088878077387</v>
+        <v>127.3401823776816</v>
       </c>
       <c r="D19" t="n">
-        <v>1.990853383650489</v>
+        <v>3.033221150684062</v>
       </c>
     </row>
     <row r="20">
@@ -1233,13 +713,13 @@
         <v>1.102040816326531</v>
       </c>
       <c r="B20" t="n">
-        <v>127.9969088572429</v>
+        <v>128.0729165228351</v>
       </c>
       <c r="C20" t="n">
-        <v>129.9904753192982</v>
+        <v>131.930072158306</v>
       </c>
       <c r="D20" t="n">
-        <v>1.993566462055298</v>
+        <v>3.011687201472605</v>
       </c>
     </row>
     <row r="21">
@@ -1247,13 +727,13 @@
         <v>1.163265306122449</v>
       </c>
       <c r="B21" t="n">
-        <v>132.5793463410754</v>
+        <v>132.6580751690689</v>
       </c>
       <c r="C21" t="n">
-        <v>134.5803984475278</v>
+        <v>136.6264514250997</v>
       </c>
       <c r="D21" t="n">
-        <v>2.001052106452448</v>
+        <v>2.991432109182346</v>
       </c>
     </row>
     <row r="22">
@@ -1261,13 +741,13 @@
         <v>1.224489795918367</v>
       </c>
       <c r="B22" t="n">
-        <v>137.2621437247731</v>
+        <v>137.343653311308</v>
       </c>
       <c r="C22" t="n">
-        <v>139.2751314329701</v>
+        <v>141.4260284907774</v>
       </c>
       <c r="D22" t="n">
-        <v>2.012987708197016</v>
+        <v>2.97237992513283</v>
       </c>
     </row>
     <row r="23">
@@ -1275,13 +755,13 @@
         <v>1.285714285714286</v>
       </c>
       <c r="B23" t="n">
-        <v>142.0423029324974</v>
+        <v>142.1266510933837</v>
       </c>
       <c r="C23" t="n">
-        <v>144.071375530439</v>
+        <v>146.3257250280111</v>
       </c>
       <c r="D23" t="n">
-        <v>2.029072597941678</v>
+        <v>2.954459211079608</v>
       </c>
     </row>
     <row r="24">
@@ -1289,13 +769,13 @@
         <v>1.346938775510204</v>
       </c>
       <c r="B24" t="n">
-        <v>146.9170184758922</v>
+        <v>147.0042613609729</v>
       </c>
       <c r="C24" t="n">
-        <v>148.9660460514896</v>
+        <v>151.3226626167132</v>
       </c>
       <c r="D24" t="n">
-        <v>2.049027575597336</v>
+        <v>2.937602771348457</v>
       </c>
     </row>
     <row r="25">
@@ -1303,13 +783,13 @@
         <v>1.408163265306122</v>
       </c>
       <c r="B25" t="n">
-        <v>151.8836648907078</v>
+        <v>151.9738570907617</v>
       </c>
       <c r="C25" t="n">
-        <v>153.9562590222412</v>
+        <v>156.4141493103249</v>
       </c>
       <c r="D25" t="n">
-        <v>2.072594131533378</v>
+        <v>2.921747400877897</v>
       </c>
     </row>
     <row r="26">
@@ -1317,13 +797,13 @@
         <v>1.469387755102041</v>
       </c>
       <c r="B26" t="n">
-        <v>156.9397843919969</v>
+        <v>157.0329790383105</v>
       </c>
       <c r="C26" t="n">
-        <v>159.0393178549598</v>
+        <v>161.5976665118064</v>
       </c>
       <c r="D26" t="n">
-        <v>2.09953346296291</v>
+        <v>2.906833648225092</v>
       </c>
     </row>
     <row r="27">
@@ -1331,13 +811,13 @@
         <v>1.530612244897959</v>
       </c>
       <c r="B27" t="n">
-        <v>162.0830749499906</v>
+        <v>162.1793238068492</v>
       </c>
       <c r="C27" t="n">
-        <v>164.2127003154827</v>
+        <v>166.870856356049</v>
       </c>
       <c r="D27" t="n">
-        <v>2.12962536549216</v>
+        <v>2.892805592645889</v>
       </c>
     </row>
     <row r="28">
@@ -1345,13 +825,13 @@
         <v>1.591836734693878</v>
       </c>
       <c r="B28" t="n">
-        <v>167.3113789185414</v>
+        <v>167.4107324689681</v>
       </c>
       <c r="C28" t="n">
-        <v>169.4740459787342</v>
+        <v>172.231509724295</v>
       </c>
       <c r="D28" t="n">
-        <v>2.162667060192859</v>
+        <v>2.879610634414076</v>
       </c>
     </row>
     <row r="29">
@@ -1359,13 +839,13 @@
         <v>1.653061224489796</v>
       </c>
       <c r="B29" t="n">
-        <v>172.6226722954507</v>
+        <v>172.7251798205668</v>
       </c>
       <c r="C29" t="n">
-        <v>174.8211442962447</v>
+        <v>177.6775549631483</v>
       </c>
       <c r="D29" t="n">
-        <v>2.198472000794055</v>
+        <v>2.86719929759298</v>
       </c>
     </row>
     <row r="30">
@@ -1373,13 +853,13 @@
         <v>1.714285714285714</v>
       </c>
       <c r="B30" t="n">
-        <v>178.0150546552689</v>
+        <v>178.120764307677</v>
       </c>
       <c r="C30" t="n">
-        <v>180.2519233484097</v>
+        <v>183.2070473419729</v>
       </c>
       <c r="D30" t="n">
-        <v>2.236868693140821</v>
+        <v>2.855525044519865</v>
       </c>
     </row>
     <row r="31">
@@ -1387,13 +867,13 @@
         <v>1.775510204081633</v>
       </c>
       <c r="B31" t="n">
-        <v>183.4867397671798</v>
+        <v>183.5956986387756</v>
       </c>
       <c r="C31" t="n">
-        <v>185.7644393165558</v>
+        <v>188.8181592546602</v>
       </c>
       <c r="D31" t="n">
-        <v>2.277699549375967</v>
+        <v>2.844544101308061</v>
       </c>
     </row>
     <row r="32">
@@ -1401,13 +881,13 @@
         <v>1.836734693877551</v>
       </c>
       <c r="B32" t="n">
-        <v>189.0360468908281</v>
+        <v>189.1483010754427</v>
       </c>
       <c r="C32" t="n">
-        <v>191.3568666827008</v>
+        <v>194.5091711523192</v>
       </c>
       <c r="D32" t="n">
-        <v>2.32081979187268</v>
+        <v>2.834215293711936</v>
       </c>
     </row>
     <row r="33">
@@ -1415,13 +895,13 @@
         <v>1.897959183673469</v>
       </c>
       <c r="B33" t="n">
-        <v>194.6613927294363</v>
+        <v>194.7769873807008</v>
       </c>
       <c r="C33" t="n">
-        <v>197.0274891457588</v>
+        <v>200.27846318035</v>
       </c>
       <c r="D33" t="n">
-        <v>2.366096416322506</v>
+        <v>2.824499892739524</v>
       </c>
     </row>
     <row r="34">
@@ -1429,13 +909,13 @@
         <v>1.959183673469388</v>
       </c>
       <c r="B34" t="n">
-        <v>200.3612840107184</v>
+        <v>200.4802633955229</v>
       </c>
       <c r="C34" t="n">
-        <v>202.7746912299196</v>
+        <v>206.1245074849802</v>
       </c>
       <c r="D34" t="n">
-        <v>2.413407219201218</v>
+        <v>2.815361469434014</v>
       </c>
     </row>
     <row r="35">
@@ -1443,13 +923,13 @@
         <v>2.020408163265306</v>
       </c>
       <c r="B35" t="n">
-        <v>206.1343106607164</v>
+        <v>206.2567182086147</v>
       </c>
       <c r="C35" t="n">
-        <v>208.5969505524873</v>
+        <v>212.0458611494448</v>
       </c>
       <c r="D35" t="n">
-        <v>2.462639891770863</v>
+        <v>2.806765758279332</v>
       </c>
     </row>
     <row r="36">
@@ -1457,13 +937,13 @@
         <v>2.081632653061225</v>
       </c>
       <c r="B36" t="n">
-        <v>211.979139532824</v>
+        <v>212.1050178817152</v>
       </c>
       <c r="C36" t="n">
-        <v>214.4928307134067</v>
+        <v>218.0411597176044</v>
       </c>
       <c r="D36" t="n">
-        <v>2.513691180582725</v>
+        <v>2.798680528717868</v>
       </c>
     </row>
     <row r="37">
@@ -1471,13 +951,13 @@
         <v>2.142857142857143</v>
       </c>
       <c r="B37" t="n">
-        <v>217.8945086532115</v>
+        <v>218.0238996916042</v>
       </c>
       <c r="C37" t="n">
-        <v>220.4609747661267</v>
+        <v>224.1091112622035</v>
       </c>
       <c r="D37" t="n">
-        <v>2.56646611291518</v>
+        <v>2.791075464298554</v>
       </c>
     </row>
     <row r="38">
@@ -1485,13 +965,13 @@
         <v>2.204081632653061</v>
       </c>
       <c r="B38" t="n">
-        <v>223.8792219440886</v>
+        <v>224.0121668502312</v>
       </c>
       <c r="C38" t="n">
-        <v>226.5000992286416</v>
+        <v>230.2484909556215</v>
       </c>
       <c r="D38" t="n">
-        <v>2.620877284552989</v>
+        <v>2.783922049001848</v>
       </c>
     </row>
     <row r="39">
@@ -1499,13 +979,13 @@
         <v>2.26530612244898</v>
       </c>
       <c r="B39" t="n">
-        <v>229.9321443873214</v>
+        <v>230.0686836654612</v>
       </c>
       <c r="C39" t="n">
-        <v>232.6089885939834</v>
+        <v>236.4581361024535</v>
       </c>
       <c r="D39" t="n">
-        <v>2.676844206661912</v>
+        <v>2.777193460316009</v>
       </c>
     </row>
     <row r="40">
@@ -1513,13 +993,13 @@
         <v>2.326530612244898</v>
       </c>
       <c r="B40" t="n">
-        <v>236.0521975925807</v>
+        <v>236.1923711065906</v>
       </c>
       <c r="C40" t="n">
-        <v>238.7864903007186</v>
+        <v>242.7369415952758</v>
       </c>
       <c r="D40" t="n">
-        <v>2.734292708137843</v>
+        <v>2.770864468663009</v>
       </c>
     </row>
     <row r="41">
@@ -1527,13 +1007,13 @@
         <v>2.387755102040816</v>
       </c>
       <c r="B41" t="n">
-        <v>242.2383557361888</v>
+        <v>242.3822027407827</v>
       </c>
       <c r="C41" t="n">
-        <v>245.0315101258265</v>
+        <v>249.0838557572852</v>
       </c>
       <c r="D41" t="n">
-        <v>2.793154389637749</v>
+        <v>2.764911342797553</v>
       </c>
     </row>
     <row r="42">
@@ -1541,13 +1021,13 @@
         <v>2.448979591836735</v>
       </c>
       <c r="B42" t="n">
-        <v>248.4896418390239</v>
+        <v>248.6372010087621</v>
       </c>
       <c r="C42" t="n">
-        <v>251.3430079644949</v>
+        <v>255.4978765379808</v>
       </c>
       <c r="D42" t="n">
-        <v>2.853366125470956</v>
+        <v>2.759311760824127</v>
       </c>
     </row>
     <row r="43">
@@ -1555,13 +1035,13 @@
         <v>2.510204081632653</v>
       </c>
       <c r="B43" t="n">
-        <v>254.8051243540962</v>
+        <v>254.9564338103635</v>
       </c>
       <c r="C43" t="n">
-        <v>257.7199939636968</v>
+        <v>261.978048030587</v>
       </c>
       <c r="D43" t="n">
-        <v>2.914869609600601</v>
+        <v>2.754044726498696</v>
       </c>
     </row>
     <row r="44">
@@ -1569,13 +1049,13 @@
         <v>2.571428571428571</v>
       </c>
       <c r="B44" t="n">
-        <v>261.1839140366615</v>
+        <v>261.3390113727879</v>
       </c>
       <c r="C44" t="n">
-        <v>264.1615249788076</v>
+        <v>268.5234572824062</v>
       </c>
       <c r="D44" t="n">
-        <v>2.977610942146043</v>
+        <v>2.749090490500878</v>
       </c>
     </row>
     <row r="45">
@@ -1583,13 +1063,13 @@
         <v>2.63265306122449</v>
       </c>
       <c r="B45" t="n">
-        <v>267.6251610719277</v>
+        <v>267.7840833766023</v>
       </c>
       <c r="C45" t="n">
-        <v>270.6667013248857</v>
+        <v>275.1332313716897</v>
       </c>
       <c r="D45" t="n">
-        <v>3.041540252957986</v>
+        <v>2.744430476381917</v>
       </c>
     </row>
     <row r="46">
@@ -1597,13 +1077,13 @@
         <v>2.693877551020408</v>
       </c>
       <c r="B46" t="n">
-        <v>274.1280524375046</v>
+        <v>274.2908363166242</v>
       </c>
       <c r="C46" t="n">
-        <v>277.2346637965524</v>
+        <v>281.8065347268993</v>
       </c>
       <c r="D46" t="n">
-        <v>3.106611359047804</v>
+        <v>2.740047210909876</v>
       </c>
     </row>
     <row r="47">
@@ -1611,13 +1091,13 @@
         <v>2.755102040816326</v>
       </c>
       <c r="B47" t="n">
-        <v>280.6918094797207</v>
+        <v>280.8584910767989</v>
       </c>
       <c r="C47" t="n">
-        <v>283.8645909325925</v>
+        <v>288.5425666663731</v>
       </c>
       <c r="D47" t="n">
-        <v>3.172781452871845</v>
+        <v>2.735924258552322</v>
       </c>
     </row>
     <row r="48">
@@ -1625,13 +1105,13 @@
         <v>2.816326530612245</v>
       </c>
       <c r="B48" t="n">
-        <v>287.3156856847787</v>
+        <v>287.4863007000309</v>
       </c>
       <c r="C48" t="n">
-        <v>290.5556965034741</v>
+        <v>295.3405591383985</v>
       </c>
       <c r="D48" t="n">
-        <v>3.240010818695453</v>
+        <v>2.732046159849157</v>
       </c>
     </row>
     <row r="49">
@@ -1639,13 +1119,13 @@
         <v>2.877551020408163</v>
       </c>
       <c r="B49" t="n">
-        <v>293.9989646274304</v>
+        <v>294.1735483356415</v>
       </c>
       <c r="C49" t="n">
-        <v>297.3072272019099</v>
+        <v>302.199774643539</v>
       </c>
       <c r="D49" t="n">
-        <v>3.308262574479556</v>
+        <v>2.728398373445822</v>
       </c>
     </row>
     <row r="50">
@@ -1653,13 +1133,13 @@
         <v>2.938775510204081</v>
       </c>
       <c r="B50" t="n">
-        <v>300.7409580814309</v>
+        <v>300.9195453487002</v>
       </c>
       <c r="C50" t="n">
-        <v>304.1184605183802</v>
+        <v>309.1195043227464</v>
       </c>
       <c r="D50" t="n">
-        <v>3.377502436949328</v>
+        <v>2.7249672215689</v>
       </c>
     </row>
     <row r="51">
@@ -1667,13 +1147,13 @@
         <v>3</v>
       </c>
       <c r="B51" t="n">
-        <v>307.5410042774784</v>
+        <v>307.7236295769306</v>
       </c>
       <c r="C51" t="n">
-        <v>310.9887027851784</v>
+        <v>316.0990661963418</v>
       </c>
       <c r="D51" t="n">
-        <v>3.447698507699954</v>
+        <v>2.721739838739724</v>
       </c>
     </row>
   </sheetData>
@@ -1681,13 +1161,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1703,182 +1183,188 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>f_sigma8_obs</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>f_sigma8_error</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
           <t>f_sigma8_LCDM</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>f_sigma8_SpinTorsion</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>f_sigma8_Observed</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>f_sigma8_Error</t>
+        </is>
+      </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Survey</t>
+          <t>Relative_Difference_Percent</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.45</v>
+        <v>0.2860720739419111</v>
       </c>
       <c r="C2" t="n">
-        <v>0.03</v>
+        <v>0.2769008360596797</v>
       </c>
       <c r="D2" t="n">
-        <v>0.47</v>
+        <v>0.2595687856150796</v>
       </c>
       <c r="E2" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>6dFGS</t>
-        </is>
+        <v>0.05</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-3.205918618988891</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.53</v>
+        <v>0.2691259211852834</v>
       </c>
       <c r="C3" t="n">
-        <v>0.04</v>
+        <v>0.2604979631694791</v>
       </c>
       <c r="D3" t="n">
-        <v>0.55</v>
+        <v>0.2524545022147803</v>
       </c>
       <c r="E3" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>SDSS</t>
-        </is>
+        <v>0.05</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-3.205918618988883</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.58</v>
+        <v>0.2539384206145838</v>
       </c>
       <c r="C4" t="n">
+        <v>0.2457973615073346</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.2230756256902471</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.05</v>
       </c>
-      <c r="D4" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>BOSS</t>
-        </is>
+      <c r="F4" t="n">
+        <v>-3.205918618988893</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.55</v>
+        <v>0.4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.65</v>
+        <v>0.2402794229162055</v>
       </c>
       <c r="C5" t="n">
-        <v>0.06</v>
+        <v>0.2325762601593358</v>
       </c>
       <c r="D5" t="n">
-        <v>0.67</v>
+        <v>0.2035813796874711</v>
       </c>
       <c r="E5" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>BOSS</t>
-        </is>
+        <v>0.05</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-3.205918618988891</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.72</v>
+        <v>0.2279483710587962</v>
       </c>
       <c r="C6" t="n">
-        <v>0.08</v>
+        <v>0.2206405317893403</v>
       </c>
       <c r="D6" t="n">
-        <v>0.73</v>
+        <v>0.1820033508915287</v>
       </c>
       <c r="E6" t="n">
-        <v>0.72</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>eBOSS</t>
-        </is>
+        <v>0.05</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-3.205918618988902</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.75</v>
+        <v>0.2167731625189172</v>
       </c>
       <c r="C7" t="n">
-        <v>0.12</v>
+        <v>0.2098235913407522</v>
       </c>
       <c r="D7" t="n">
-        <v>0.76</v>
+        <v>0.2191354694131956</v>
       </c>
       <c r="E7" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>eBOSS</t>
-        </is>
+        <v>0.05</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-3.205918618988896</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.78</v>
+        <v>0.1973252059590575</v>
       </c>
       <c r="C8" t="n">
-        <v>0.15</v>
+        <v>0.1909991204412579</v>
       </c>
       <c r="D8" t="n">
-        <v>0.79</v>
+        <v>0.2110966957461885</v>
       </c>
       <c r="E8" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>eBOSS</t>
-        </is>
+        <v>0.05</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-3.205918618988899</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.1810042336763583</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1752013852477697</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.1788702808662465</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-3.205918618988888</v>
       </c>
     </row>
   </sheetData>

</xml_diff>